<commit_message>
Ajout des données AFNIC
</commit_message>
<xml_diff>
--- a/Data/Import-KUMU-SitesWeb-AdministrationsPubliques.xlsx
+++ b/Data/Import-KUMU-SitesWeb-AdministrationsPubliques.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="-26180" yWindow="3000" windowWidth="25120" windowHeight="15580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Elements" sheetId="3" r:id="rId1"/>
@@ -12,7 +12,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Connections!$A$1:$E$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Elements!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Elements!$A$1:$F$588</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3507" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3921" uniqueCount="684">
   <si>
     <t>http://www.culture.gouv.fr</t>
   </si>
@@ -1872,6 +1872,210 @@
   </si>
   <si>
     <t>http://telepac.agriculture.gouv.fr</t>
+  </si>
+  <si>
+    <t>https://monavis.numerique.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://prefectures-regions.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://aisne.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://alpes-de-haute-provence.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://alpes-maritimes.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://ariege.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://aube.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://bas-rhin.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://bouches-du-rhone.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://charente.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://charente-maritime.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://cher.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://correze.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://cotes-darmor.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://creuse.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://dordogne.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://essonne.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://eure-et-loir.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://eure.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://finistere.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://gers.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://guadeloupe.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://guyane.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://haute-garonne.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://haute-marne.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://haute-saone.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://haute-savoie.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://haute-vienne.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://haut-rhin.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://hauts-de-seine.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://herault.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://ille-et-vilaine.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://indre-et-loire.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://indre.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://isere.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://jura.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://loire-atlantique.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://loir-et-cher.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://loiret.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://lozere.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://manche.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://mayenne.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://mayotte.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://meurthe-et-moselle.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://meuse.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://morbihan.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://moselle.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://nord.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://nouvelle-caledonie.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://oise.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://pas-de-calais.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://pyrenees-atlantiques.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://pyrenees-orientales.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://rhone.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://saint-barth-saint-martin.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://saint-pierre-et-miquelon.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://savoie.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://seine-et-marne.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://seine-maritime.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://seine-saint-denis.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://somme.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://tarn-et-garonne.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://territoire-de-belfort.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://val-de-marne.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://val-doise.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://vienne.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://vosges.gouv.fr</t>
+  </si>
+  <si>
+    <t>http://yvelines.gouv.fr</t>
   </si>
 </sst>
 </file>
@@ -1940,7 +2144,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2558">
+  <cellStyleXfs count="2770">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4314,6 +4518,218 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4506,7 +4922,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2558">
+  <cellStyles count="2770">
     <cellStyle name="Lien hypertexte" xfId="64" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="66" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="68" builtinId="8" hidden="1"/>
@@ -5382,6 +5798,112 @@
     <cellStyle name="Lien hypertexte" xfId="2552" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="2554" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="2556" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2558" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2560" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2562" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2564" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2566" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2568" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2570" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2572" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2574" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2576" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2578" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2580" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2582" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2584" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2586" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2588" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2590" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2592" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2594" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2596" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2598" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2600" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2602" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2604" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2606" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2608" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2610" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2612" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2614" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2616" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2618" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2620" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2622" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2624" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2626" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2628" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2630" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2632" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2634" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2636" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2638" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2640" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2642" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2644" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2646" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2648" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2650" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2652" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2654" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2656" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2658" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2660" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2662" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2664" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2666" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2668" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2670" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2672" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2674" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2676" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2678" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2680" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2682" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2684" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2686" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2688" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2690" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2692" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2694" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2696" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2698" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2700" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2702" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2704" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2706" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2708" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2710" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2712" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2714" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2716" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2718" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2720" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2722" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2724" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2726" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2728" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2730" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2732" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2734" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2736" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2738" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2740" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2742" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2744" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2746" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2748" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2750" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2752" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2754" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2756" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2758" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2760" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2762" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2764" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2766" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="2768" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte 2" xfId="2226"/>
     <cellStyle name="Lien hypertexte visité" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
@@ -7064,9 +7586,155 @@
     <cellStyle name="Lien hypertexte visité" xfId="2553" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2555" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2557" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2559" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2561" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2563" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2565" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2567" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2569" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2571" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2573" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2575" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2577" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2579" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2581" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2583" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2585" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2587" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2589" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2591" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2593" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2595" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2597" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2599" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2601" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2603" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2605" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2607" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2609" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2611" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2613" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2615" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2617" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2619" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2621" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2623" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2625" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2627" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2629" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2631" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2633" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2635" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2637" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2639" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2641" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2643" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2645" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2647" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2649" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2651" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2653" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2655" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2657" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2659" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2661" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2663" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2665" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2667" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2669" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2671" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2673" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2675" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2677" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2679" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2681" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2683" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2685" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2687" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2689" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2691" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2693" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2695" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2697" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2699" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2701" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2703" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2705" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2707" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2709" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2711" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2713" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2715" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2717" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2719" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2721" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2723" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2725" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2727" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2729" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2731" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2733" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2735" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2737" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2739" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2741" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2743" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2745" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2747" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2749" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2751" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2753" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2755" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2757" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2759" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2761" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2763" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2765" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2767" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2769" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="334">
+  <dxfs count="338">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -10734,10 +11402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F588"/>
+  <dimension ref="A1:F657"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B514" sqref="B514"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10999,7 +11667,7 @@
         <v>569</v>
       </c>
       <c r="E18">
-        <v>32</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -11027,7 +11695,7 @@
         <v>33</v>
       </c>
       <c r="E20">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -17383,69 +18051,828 @@
         <v>589</v>
       </c>
     </row>
+    <row r="589" spans="1:4">
+      <c r="A589" t="s">
+        <v>616</v>
+      </c>
+      <c r="B589" t="s">
+        <v>552</v>
+      </c>
+      <c r="D589" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="590" spans="1:4">
+      <c r="A590" t="s">
+        <v>617</v>
+      </c>
+      <c r="B590" t="s">
+        <v>552</v>
+      </c>
+      <c r="D590" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="591" spans="1:4">
+      <c r="A591" t="s">
+        <v>618</v>
+      </c>
+      <c r="B591" t="s">
+        <v>552</v>
+      </c>
+      <c r="D591" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="592" spans="1:4">
+      <c r="A592" t="s">
+        <v>619</v>
+      </c>
+      <c r="B592" t="s">
+        <v>552</v>
+      </c>
+      <c r="D592" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="593" spans="1:4">
+      <c r="A593" t="s">
+        <v>620</v>
+      </c>
+      <c r="B593" t="s">
+        <v>552</v>
+      </c>
+      <c r="D593" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="594" spans="1:4">
+      <c r="A594" t="s">
+        <v>621</v>
+      </c>
+      <c r="B594" t="s">
+        <v>552</v>
+      </c>
+      <c r="D594" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="595" spans="1:4">
+      <c r="A595" t="s">
+        <v>622</v>
+      </c>
+      <c r="B595" t="s">
+        <v>552</v>
+      </c>
+      <c r="D595" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="596" spans="1:4">
+      <c r="A596" t="s">
+        <v>623</v>
+      </c>
+      <c r="B596" t="s">
+        <v>552</v>
+      </c>
+      <c r="D596" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="597" spans="1:4">
+      <c r="A597" t="s">
+        <v>624</v>
+      </c>
+      <c r="B597" t="s">
+        <v>552</v>
+      </c>
+      <c r="D597" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="598" spans="1:4">
+      <c r="A598" t="s">
+        <v>625</v>
+      </c>
+      <c r="B598" t="s">
+        <v>552</v>
+      </c>
+      <c r="D598" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="599" spans="1:4">
+      <c r="A599" t="s">
+        <v>626</v>
+      </c>
+      <c r="B599" t="s">
+        <v>552</v>
+      </c>
+      <c r="D599" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="600" spans="1:4">
+      <c r="A600" t="s">
+        <v>627</v>
+      </c>
+      <c r="B600" t="s">
+        <v>552</v>
+      </c>
+      <c r="D600" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="601" spans="1:4">
+      <c r="A601" t="s">
+        <v>628</v>
+      </c>
+      <c r="B601" t="s">
+        <v>552</v>
+      </c>
+      <c r="D601" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="602" spans="1:4">
+      <c r="A602" t="s">
+        <v>629</v>
+      </c>
+      <c r="B602" t="s">
+        <v>552</v>
+      </c>
+      <c r="D602" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="603" spans="1:4">
+      <c r="A603" t="s">
+        <v>630</v>
+      </c>
+      <c r="B603" t="s">
+        <v>552</v>
+      </c>
+      <c r="D603" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="604" spans="1:4">
+      <c r="A604" t="s">
+        <v>631</v>
+      </c>
+      <c r="B604" t="s">
+        <v>552</v>
+      </c>
+      <c r="D604" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="605" spans="1:4">
+      <c r="A605" t="s">
+        <v>632</v>
+      </c>
+      <c r="B605" t="s">
+        <v>552</v>
+      </c>
+      <c r="D605" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="606" spans="1:4">
+      <c r="A606" t="s">
+        <v>633</v>
+      </c>
+      <c r="B606" t="s">
+        <v>552</v>
+      </c>
+      <c r="D606" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="607" spans="1:4">
+      <c r="A607" t="s">
+        <v>634</v>
+      </c>
+      <c r="B607" t="s">
+        <v>552</v>
+      </c>
+      <c r="D607" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="608" spans="1:4">
+      <c r="A608" t="s">
+        <v>635</v>
+      </c>
+      <c r="B608" t="s">
+        <v>552</v>
+      </c>
+      <c r="D608" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="609" spans="1:4">
+      <c r="A609" t="s">
+        <v>636</v>
+      </c>
+      <c r="B609" t="s">
+        <v>552</v>
+      </c>
+      <c r="D609" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="610" spans="1:4">
+      <c r="A610" t="s">
+        <v>637</v>
+      </c>
+      <c r="B610" t="s">
+        <v>552</v>
+      </c>
+      <c r="D610" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="611" spans="1:4">
+      <c r="A611" t="s">
+        <v>638</v>
+      </c>
+      <c r="B611" t="s">
+        <v>552</v>
+      </c>
+      <c r="D611" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="612" spans="1:4">
+      <c r="A612" t="s">
+        <v>639</v>
+      </c>
+      <c r="B612" t="s">
+        <v>552</v>
+      </c>
+      <c r="D612" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="613" spans="1:4">
+      <c r="A613" t="s">
+        <v>640</v>
+      </c>
+      <c r="B613" t="s">
+        <v>552</v>
+      </c>
+      <c r="D613" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="614" spans="1:4">
+      <c r="A614" t="s">
+        <v>641</v>
+      </c>
+      <c r="B614" t="s">
+        <v>552</v>
+      </c>
+      <c r="D614" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="615" spans="1:4">
+      <c r="A615" t="s">
+        <v>642</v>
+      </c>
+      <c r="B615" t="s">
+        <v>552</v>
+      </c>
+      <c r="D615" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="616" spans="1:4">
+      <c r="A616" t="s">
+        <v>643</v>
+      </c>
+      <c r="B616" t="s">
+        <v>552</v>
+      </c>
+      <c r="D616" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="617" spans="1:4">
+      <c r="A617" t="s">
+        <v>644</v>
+      </c>
+      <c r="B617" t="s">
+        <v>552</v>
+      </c>
+      <c r="D617" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="618" spans="1:4">
+      <c r="A618" t="s">
+        <v>645</v>
+      </c>
+      <c r="B618" t="s">
+        <v>552</v>
+      </c>
+      <c r="D618" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="619" spans="1:4">
+      <c r="A619" t="s">
+        <v>646</v>
+      </c>
+      <c r="B619" t="s">
+        <v>552</v>
+      </c>
+      <c r="D619" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="620" spans="1:4">
+      <c r="A620" t="s">
+        <v>647</v>
+      </c>
+      <c r="B620" t="s">
+        <v>552</v>
+      </c>
+      <c r="D620" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="621" spans="1:4">
+      <c r="A621" t="s">
+        <v>648</v>
+      </c>
+      <c r="B621" t="s">
+        <v>552</v>
+      </c>
+      <c r="D621" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="622" spans="1:4">
+      <c r="A622" t="s">
+        <v>649</v>
+      </c>
+      <c r="B622" t="s">
+        <v>552</v>
+      </c>
+      <c r="D622" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="623" spans="1:4">
+      <c r="A623" t="s">
+        <v>650</v>
+      </c>
+      <c r="B623" t="s">
+        <v>552</v>
+      </c>
+      <c r="D623" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="624" spans="1:4">
+      <c r="A624" t="s">
+        <v>651</v>
+      </c>
+      <c r="B624" t="s">
+        <v>552</v>
+      </c>
+      <c r="D624" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="625" spans="1:4">
+      <c r="A625" t="s">
+        <v>652</v>
+      </c>
+      <c r="B625" t="s">
+        <v>552</v>
+      </c>
+      <c r="D625" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="626" spans="1:4">
+      <c r="A626" t="s">
+        <v>653</v>
+      </c>
+      <c r="B626" t="s">
+        <v>552</v>
+      </c>
+      <c r="D626" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="627" spans="1:4">
+      <c r="A627" t="s">
+        <v>654</v>
+      </c>
+      <c r="B627" t="s">
+        <v>552</v>
+      </c>
+      <c r="D627" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="628" spans="1:4">
+      <c r="A628" t="s">
+        <v>655</v>
+      </c>
+      <c r="B628" t="s">
+        <v>552</v>
+      </c>
+      <c r="D628" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="629" spans="1:4">
+      <c r="A629" t="s">
+        <v>656</v>
+      </c>
+      <c r="B629" t="s">
+        <v>552</v>
+      </c>
+      <c r="D629" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="630" spans="1:4">
+      <c r="A630" t="s">
+        <v>657</v>
+      </c>
+      <c r="B630" t="s">
+        <v>552</v>
+      </c>
+      <c r="D630" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="631" spans="1:4">
+      <c r="A631" t="s">
+        <v>658</v>
+      </c>
+      <c r="B631" t="s">
+        <v>552</v>
+      </c>
+      <c r="D631" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="632" spans="1:4">
+      <c r="A632" t="s">
+        <v>659</v>
+      </c>
+      <c r="B632" t="s">
+        <v>552</v>
+      </c>
+      <c r="D632" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="633" spans="1:4">
+      <c r="A633" t="s">
+        <v>660</v>
+      </c>
+      <c r="B633" t="s">
+        <v>552</v>
+      </c>
+      <c r="D633" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="634" spans="1:4">
+      <c r="A634" t="s">
+        <v>661</v>
+      </c>
+      <c r="B634" t="s">
+        <v>552</v>
+      </c>
+      <c r="D634" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="635" spans="1:4">
+      <c r="A635" t="s">
+        <v>662</v>
+      </c>
+      <c r="B635" t="s">
+        <v>552</v>
+      </c>
+      <c r="D635" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="636" spans="1:4">
+      <c r="A636" t="s">
+        <v>663</v>
+      </c>
+      <c r="B636" t="s">
+        <v>552</v>
+      </c>
+      <c r="D636" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="637" spans="1:4">
+      <c r="A637" t="s">
+        <v>664</v>
+      </c>
+      <c r="B637" t="s">
+        <v>552</v>
+      </c>
+      <c r="D637" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="638" spans="1:4">
+      <c r="A638" t="s">
+        <v>665</v>
+      </c>
+      <c r="B638" t="s">
+        <v>552</v>
+      </c>
+      <c r="D638" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="639" spans="1:4">
+      <c r="A639" t="s">
+        <v>666</v>
+      </c>
+      <c r="B639" t="s">
+        <v>552</v>
+      </c>
+      <c r="D639" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="640" spans="1:4">
+      <c r="A640" t="s">
+        <v>617</v>
+      </c>
+      <c r="B640" t="s">
+        <v>552</v>
+      </c>
+      <c r="D640" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="641" spans="1:4">
+      <c r="A641" t="s">
+        <v>667</v>
+      </c>
+      <c r="B641" t="s">
+        <v>552</v>
+      </c>
+      <c r="D641" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="642" spans="1:4">
+      <c r="A642" t="s">
+        <v>668</v>
+      </c>
+      <c r="B642" t="s">
+        <v>552</v>
+      </c>
+      <c r="D642" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="643" spans="1:4">
+      <c r="A643" t="s">
+        <v>669</v>
+      </c>
+      <c r="B643" t="s">
+        <v>552</v>
+      </c>
+      <c r="D643" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="644" spans="1:4">
+      <c r="A644" t="s">
+        <v>670</v>
+      </c>
+      <c r="B644" t="s">
+        <v>552</v>
+      </c>
+      <c r="D644" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="645" spans="1:4">
+      <c r="A645" t="s">
+        <v>671</v>
+      </c>
+      <c r="B645" t="s">
+        <v>552</v>
+      </c>
+      <c r="D645" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="646" spans="1:4">
+      <c r="A646" t="s">
+        <v>672</v>
+      </c>
+      <c r="B646" t="s">
+        <v>552</v>
+      </c>
+      <c r="D646" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="647" spans="1:4">
+      <c r="A647" t="s">
+        <v>673</v>
+      </c>
+      <c r="B647" t="s">
+        <v>552</v>
+      </c>
+      <c r="D647" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="648" spans="1:4">
+      <c r="A648" t="s">
+        <v>674</v>
+      </c>
+      <c r="B648" t="s">
+        <v>552</v>
+      </c>
+      <c r="D648" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="649" spans="1:4">
+      <c r="A649" t="s">
+        <v>675</v>
+      </c>
+      <c r="B649" t="s">
+        <v>552</v>
+      </c>
+      <c r="D649" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="650" spans="1:4">
+      <c r="A650" t="s">
+        <v>676</v>
+      </c>
+      <c r="B650" t="s">
+        <v>552</v>
+      </c>
+      <c r="D650" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="651" spans="1:4">
+      <c r="A651" t="s">
+        <v>677</v>
+      </c>
+      <c r="B651" t="s">
+        <v>552</v>
+      </c>
+      <c r="D651" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="652" spans="1:4">
+      <c r="A652" t="s">
+        <v>678</v>
+      </c>
+      <c r="B652" t="s">
+        <v>552</v>
+      </c>
+      <c r="D652" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="653" spans="1:4">
+      <c r="A653" t="s">
+        <v>679</v>
+      </c>
+      <c r="B653" t="s">
+        <v>552</v>
+      </c>
+      <c r="D653" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="654" spans="1:4">
+      <c r="A654" t="s">
+        <v>680</v>
+      </c>
+      <c r="B654" t="s">
+        <v>552</v>
+      </c>
+      <c r="D654" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="655" spans="1:4">
+      <c r="A655" t="s">
+        <v>681</v>
+      </c>
+      <c r="B655" t="s">
+        <v>552</v>
+      </c>
+      <c r="D655" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="656" spans="1:4">
+      <c r="A656" t="s">
+        <v>682</v>
+      </c>
+      <c r="B656" t="s">
+        <v>552</v>
+      </c>
+      <c r="D656" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="657" spans="1:4">
+      <c r="A657" t="s">
+        <v>683</v>
+      </c>
+      <c r="B657" t="s">
+        <v>552</v>
+      </c>
+      <c r="D657" t="s">
+        <v>552</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F1"/>
-  <conditionalFormatting sqref="A395:A566 A22:A371 A373:A377 A379 A381:A393 A1:A3 A576:A577 A579 A584 A587:A1048576">
-    <cfRule type="duplicateValues" dxfId="333" priority="13"/>
-    <cfRule type="duplicateValues" dxfId="332" priority="14"/>
+  <autoFilter ref="A1:F588"/>
+  <conditionalFormatting sqref="A395:A566 A22:A371 A373:A377 A379 A381:A393 A1:A3 A576:A577 A579 A584 A587:A590 A658:A1048576">
+    <cfRule type="duplicateValues" dxfId="337" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="336" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F427 F1 F539 F514 F517 B533:D533 B429:C429 B470:C470 B430:D469 B1:D428 B471:D531 B537:D556 B558:D1048576">
-    <cfRule type="containsText" dxfId="331" priority="12" operator="containsText" text="Non">
+    <cfRule type="containsText" dxfId="335" priority="12" operator="containsText" text="Non">
       <formula>NOT(ISERROR(SEARCH("Non",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F471">
-    <cfRule type="containsText" dxfId="330" priority="11" operator="containsText" text="Non">
+    <cfRule type="containsText" dxfId="334" priority="11" operator="containsText" text="Non">
       <formula>NOT(ISERROR(SEARCH("Non",F471)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F500">
-    <cfRule type="containsText" dxfId="329" priority="10" operator="containsText" text="Non">
+    <cfRule type="containsText" dxfId="333" priority="10" operator="containsText" text="Non">
       <formula>NOT(ISERROR(SEARCH("Non",F500)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22">
-    <cfRule type="containsText" dxfId="328" priority="9" operator="containsText" text="Non">
+    <cfRule type="containsText" dxfId="332" priority="9" operator="containsText" text="Non">
       <formula>NOT(ISERROR(SEARCH("Non",F22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F495">
-    <cfRule type="containsText" dxfId="327" priority="8" operator="containsText" text="Non">
+    <cfRule type="containsText" dxfId="331" priority="8" operator="containsText" text="Non">
       <formula>NOT(ISERROR(SEARCH("Non",F495)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F513">
-    <cfRule type="containsText" dxfId="326" priority="7" operator="containsText" text="Non">
+    <cfRule type="containsText" dxfId="330" priority="7" operator="containsText" text="Non">
       <formula>NOT(ISERROR(SEARCH("Non",F513)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F518">
-    <cfRule type="containsText" dxfId="325" priority="6" operator="containsText" text="Non">
+    <cfRule type="containsText" dxfId="329" priority="6" operator="containsText" text="Non">
       <formula>NOT(ISERROR(SEARCH("Non",F518)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B532:D532">
-    <cfRule type="containsText" dxfId="324" priority="5" operator="containsText" text="Non">
+    <cfRule type="containsText" dxfId="328" priority="5" operator="containsText" text="Non">
       <formula>NOT(ISERROR(SEARCH("Non",B532)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B534:D534">
-    <cfRule type="containsText" dxfId="323" priority="4" operator="containsText" text="Non">
+    <cfRule type="containsText" dxfId="327" priority="4" operator="containsText" text="Non">
       <formula>NOT(ISERROR(SEARCH("Non",B534)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B535:D535">
-    <cfRule type="containsText" dxfId="322" priority="3" operator="containsText" text="Non">
+    <cfRule type="containsText" dxfId="326" priority="3" operator="containsText" text="Non">
       <formula>NOT(ISERROR(SEARCH("Non",B535)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B536:D536">
-    <cfRule type="containsText" dxfId="321" priority="2" operator="containsText" text="Non">
+    <cfRule type="containsText" dxfId="325" priority="2" operator="containsText" text="Non">
       <formula>NOT(ISERROR(SEARCH("Non",B536)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B557:D557">
-    <cfRule type="containsText" dxfId="320" priority="1" operator="containsText" text="Non">
+    <cfRule type="containsText" dxfId="324" priority="1" operator="containsText" text="Non">
       <formula>NOT(ISERROR(SEARCH("Non",B557)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17460,10 +18887,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E578"/>
+  <dimension ref="A1:E647"/>
   <sheetViews>
-    <sheetView topLeftCell="A352" workbookViewId="0">
-      <selection activeCell="A339" sqref="A339:A358"/>
+    <sheetView topLeftCell="A614" workbookViewId="0">
+      <selection activeCell="A581" sqref="A581:A647"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -23850,6 +25277,765 @@
         <v>564</v>
       </c>
     </row>
+    <row r="579" spans="1:3">
+      <c r="A579" t="s">
+        <v>526</v>
+      </c>
+      <c r="B579" t="s">
+        <v>616</v>
+      </c>
+      <c r="C579" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="580" spans="1:3">
+      <c r="A580" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B580" t="s">
+        <v>617</v>
+      </c>
+      <c r="C580" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="581" spans="1:3">
+      <c r="A581" t="s">
+        <v>553</v>
+      </c>
+      <c r="B581" t="s">
+        <v>618</v>
+      </c>
+      <c r="C581" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="582" spans="1:3">
+      <c r="A582" t="s">
+        <v>553</v>
+      </c>
+      <c r="B582" t="s">
+        <v>619</v>
+      </c>
+      <c r="C582" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="583" spans="1:3">
+      <c r="A583" t="s">
+        <v>553</v>
+      </c>
+      <c r="B583" t="s">
+        <v>620</v>
+      </c>
+      <c r="C583" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="584" spans="1:3">
+      <c r="A584" t="s">
+        <v>553</v>
+      </c>
+      <c r="B584" t="s">
+        <v>621</v>
+      </c>
+      <c r="C584" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="585" spans="1:3">
+      <c r="A585" t="s">
+        <v>553</v>
+      </c>
+      <c r="B585" t="s">
+        <v>622</v>
+      </c>
+      <c r="C585" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="586" spans="1:3">
+      <c r="A586" t="s">
+        <v>553</v>
+      </c>
+      <c r="B586" t="s">
+        <v>623</v>
+      </c>
+      <c r="C586" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="587" spans="1:3">
+      <c r="A587" t="s">
+        <v>553</v>
+      </c>
+      <c r="B587" t="s">
+        <v>624</v>
+      </c>
+      <c r="C587" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="588" spans="1:3">
+      <c r="A588" t="s">
+        <v>553</v>
+      </c>
+      <c r="B588" t="s">
+        <v>625</v>
+      </c>
+      <c r="C588" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="589" spans="1:3">
+      <c r="A589" t="s">
+        <v>553</v>
+      </c>
+      <c r="B589" t="s">
+        <v>626</v>
+      </c>
+      <c r="C589" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="590" spans="1:3">
+      <c r="A590" t="s">
+        <v>553</v>
+      </c>
+      <c r="B590" t="s">
+        <v>627</v>
+      </c>
+      <c r="C590" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="591" spans="1:3">
+      <c r="A591" t="s">
+        <v>553</v>
+      </c>
+      <c r="B591" t="s">
+        <v>628</v>
+      </c>
+      <c r="C591" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="592" spans="1:3">
+      <c r="A592" t="s">
+        <v>553</v>
+      </c>
+      <c r="B592" t="s">
+        <v>629</v>
+      </c>
+      <c r="C592" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="593" spans="1:3">
+      <c r="A593" t="s">
+        <v>553</v>
+      </c>
+      <c r="B593" t="s">
+        <v>630</v>
+      </c>
+      <c r="C593" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="594" spans="1:3">
+      <c r="A594" t="s">
+        <v>553</v>
+      </c>
+      <c r="B594" t="s">
+        <v>631</v>
+      </c>
+      <c r="C594" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="595" spans="1:3">
+      <c r="A595" t="s">
+        <v>553</v>
+      </c>
+      <c r="B595" t="s">
+        <v>632</v>
+      </c>
+      <c r="C595" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="596" spans="1:3">
+      <c r="A596" t="s">
+        <v>553</v>
+      </c>
+      <c r="B596" t="s">
+        <v>633</v>
+      </c>
+      <c r="C596" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="597" spans="1:3">
+      <c r="A597" t="s">
+        <v>553</v>
+      </c>
+      <c r="B597" t="s">
+        <v>634</v>
+      </c>
+      <c r="C597" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="598" spans="1:3">
+      <c r="A598" t="s">
+        <v>553</v>
+      </c>
+      <c r="B598" t="s">
+        <v>635</v>
+      </c>
+      <c r="C598" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="599" spans="1:3">
+      <c r="A599" t="s">
+        <v>553</v>
+      </c>
+      <c r="B599" t="s">
+        <v>636</v>
+      </c>
+      <c r="C599" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="600" spans="1:3">
+      <c r="A600" t="s">
+        <v>553</v>
+      </c>
+      <c r="B600" t="s">
+        <v>637</v>
+      </c>
+      <c r="C600" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="601" spans="1:3">
+      <c r="A601" t="s">
+        <v>553</v>
+      </c>
+      <c r="B601" t="s">
+        <v>638</v>
+      </c>
+      <c r="C601" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="602" spans="1:3">
+      <c r="A602" t="s">
+        <v>553</v>
+      </c>
+      <c r="B602" t="s">
+        <v>639</v>
+      </c>
+      <c r="C602" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="603" spans="1:3">
+      <c r="A603" t="s">
+        <v>553</v>
+      </c>
+      <c r="B603" t="s">
+        <v>640</v>
+      </c>
+      <c r="C603" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="604" spans="1:3">
+      <c r="A604" t="s">
+        <v>553</v>
+      </c>
+      <c r="B604" t="s">
+        <v>641</v>
+      </c>
+      <c r="C604" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="605" spans="1:3">
+      <c r="A605" t="s">
+        <v>553</v>
+      </c>
+      <c r="B605" t="s">
+        <v>642</v>
+      </c>
+      <c r="C605" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="606" spans="1:3">
+      <c r="A606" t="s">
+        <v>553</v>
+      </c>
+      <c r="B606" t="s">
+        <v>643</v>
+      </c>
+      <c r="C606" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="607" spans="1:3">
+      <c r="A607" t="s">
+        <v>553</v>
+      </c>
+      <c r="B607" t="s">
+        <v>644</v>
+      </c>
+      <c r="C607" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="608" spans="1:3">
+      <c r="A608" t="s">
+        <v>553</v>
+      </c>
+      <c r="B608" t="s">
+        <v>645</v>
+      </c>
+      <c r="C608" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="609" spans="1:3">
+      <c r="A609" t="s">
+        <v>553</v>
+      </c>
+      <c r="B609" t="s">
+        <v>646</v>
+      </c>
+      <c r="C609" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="610" spans="1:3">
+      <c r="A610" t="s">
+        <v>553</v>
+      </c>
+      <c r="B610" t="s">
+        <v>647</v>
+      </c>
+      <c r="C610" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="611" spans="1:3">
+      <c r="A611" t="s">
+        <v>553</v>
+      </c>
+      <c r="B611" t="s">
+        <v>648</v>
+      </c>
+      <c r="C611" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="612" spans="1:3">
+      <c r="A612" t="s">
+        <v>553</v>
+      </c>
+      <c r="B612" t="s">
+        <v>649</v>
+      </c>
+      <c r="C612" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="613" spans="1:3">
+      <c r="A613" t="s">
+        <v>553</v>
+      </c>
+      <c r="B613" t="s">
+        <v>650</v>
+      </c>
+      <c r="C613" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="614" spans="1:3">
+      <c r="A614" t="s">
+        <v>553</v>
+      </c>
+      <c r="B614" t="s">
+        <v>651</v>
+      </c>
+      <c r="C614" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="615" spans="1:3">
+      <c r="A615" t="s">
+        <v>553</v>
+      </c>
+      <c r="B615" t="s">
+        <v>652</v>
+      </c>
+      <c r="C615" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="616" spans="1:3">
+      <c r="A616" t="s">
+        <v>553</v>
+      </c>
+      <c r="B616" t="s">
+        <v>653</v>
+      </c>
+      <c r="C616" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="617" spans="1:3">
+      <c r="A617" t="s">
+        <v>553</v>
+      </c>
+      <c r="B617" t="s">
+        <v>654</v>
+      </c>
+      <c r="C617" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="618" spans="1:3">
+      <c r="A618" t="s">
+        <v>553</v>
+      </c>
+      <c r="B618" t="s">
+        <v>655</v>
+      </c>
+      <c r="C618" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="619" spans="1:3">
+      <c r="A619" t="s">
+        <v>553</v>
+      </c>
+      <c r="B619" t="s">
+        <v>656</v>
+      </c>
+      <c r="C619" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="620" spans="1:3">
+      <c r="A620" t="s">
+        <v>553</v>
+      </c>
+      <c r="B620" t="s">
+        <v>657</v>
+      </c>
+      <c r="C620" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="621" spans="1:3">
+      <c r="A621" t="s">
+        <v>553</v>
+      </c>
+      <c r="B621" t="s">
+        <v>658</v>
+      </c>
+      <c r="C621" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="622" spans="1:3">
+      <c r="A622" t="s">
+        <v>553</v>
+      </c>
+      <c r="B622" t="s">
+        <v>659</v>
+      </c>
+      <c r="C622" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="623" spans="1:3">
+      <c r="A623" t="s">
+        <v>553</v>
+      </c>
+      <c r="B623" t="s">
+        <v>660</v>
+      </c>
+      <c r="C623" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="624" spans="1:3">
+      <c r="A624" t="s">
+        <v>553</v>
+      </c>
+      <c r="B624" t="s">
+        <v>661</v>
+      </c>
+      <c r="C624" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="625" spans="1:3">
+      <c r="A625" t="s">
+        <v>553</v>
+      </c>
+      <c r="B625" t="s">
+        <v>662</v>
+      </c>
+      <c r="C625" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="626" spans="1:3">
+      <c r="A626" t="s">
+        <v>553</v>
+      </c>
+      <c r="B626" t="s">
+        <v>663</v>
+      </c>
+      <c r="C626" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="627" spans="1:3">
+      <c r="A627" t="s">
+        <v>553</v>
+      </c>
+      <c r="B627" t="s">
+        <v>664</v>
+      </c>
+      <c r="C627" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="628" spans="1:3">
+      <c r="A628" t="s">
+        <v>553</v>
+      </c>
+      <c r="B628" t="s">
+        <v>665</v>
+      </c>
+      <c r="C628" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="629" spans="1:3">
+      <c r="A629" t="s">
+        <v>553</v>
+      </c>
+      <c r="B629" t="s">
+        <v>666</v>
+      </c>
+      <c r="C629" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="630" spans="1:3">
+      <c r="A630" t="s">
+        <v>553</v>
+      </c>
+      <c r="B630" t="s">
+        <v>617</v>
+      </c>
+      <c r="C630" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="631" spans="1:3">
+      <c r="A631" t="s">
+        <v>553</v>
+      </c>
+      <c r="B631" t="s">
+        <v>667</v>
+      </c>
+      <c r="C631" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="632" spans="1:3">
+      <c r="A632" t="s">
+        <v>553</v>
+      </c>
+      <c r="B632" t="s">
+        <v>668</v>
+      </c>
+      <c r="C632" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="633" spans="1:3">
+      <c r="A633" t="s">
+        <v>553</v>
+      </c>
+      <c r="B633" t="s">
+        <v>669</v>
+      </c>
+      <c r="C633" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="634" spans="1:3">
+      <c r="A634" t="s">
+        <v>553</v>
+      </c>
+      <c r="B634" t="s">
+        <v>670</v>
+      </c>
+      <c r="C634" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="635" spans="1:3">
+      <c r="A635" t="s">
+        <v>553</v>
+      </c>
+      <c r="B635" t="s">
+        <v>671</v>
+      </c>
+      <c r="C635" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="636" spans="1:3">
+      <c r="A636" t="s">
+        <v>553</v>
+      </c>
+      <c r="B636" t="s">
+        <v>672</v>
+      </c>
+      <c r="C636" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="637" spans="1:3">
+      <c r="A637" t="s">
+        <v>553</v>
+      </c>
+      <c r="B637" t="s">
+        <v>673</v>
+      </c>
+      <c r="C637" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="638" spans="1:3">
+      <c r="A638" t="s">
+        <v>553</v>
+      </c>
+      <c r="B638" t="s">
+        <v>674</v>
+      </c>
+      <c r="C638" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="639" spans="1:3">
+      <c r="A639" t="s">
+        <v>553</v>
+      </c>
+      <c r="B639" t="s">
+        <v>675</v>
+      </c>
+      <c r="C639" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="640" spans="1:3">
+      <c r="A640" t="s">
+        <v>553</v>
+      </c>
+      <c r="B640" t="s">
+        <v>676</v>
+      </c>
+      <c r="C640" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="641" spans="1:3">
+      <c r="A641" t="s">
+        <v>553</v>
+      </c>
+      <c r="B641" t="s">
+        <v>677</v>
+      </c>
+      <c r="C641" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="642" spans="1:3">
+      <c r="A642" t="s">
+        <v>553</v>
+      </c>
+      <c r="B642" t="s">
+        <v>678</v>
+      </c>
+      <c r="C642" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="643" spans="1:3">
+      <c r="A643" t="s">
+        <v>553</v>
+      </c>
+      <c r="B643" t="s">
+        <v>679</v>
+      </c>
+      <c r="C643" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="644" spans="1:3">
+      <c r="A644" t="s">
+        <v>553</v>
+      </c>
+      <c r="B644" t="s">
+        <v>680</v>
+      </c>
+      <c r="C644" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="645" spans="1:3">
+      <c r="A645" t="s">
+        <v>553</v>
+      </c>
+      <c r="B645" t="s">
+        <v>681</v>
+      </c>
+      <c r="C645" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="646" spans="1:3">
+      <c r="A646" t="s">
+        <v>553</v>
+      </c>
+      <c r="B646" t="s">
+        <v>682</v>
+      </c>
+      <c r="C646" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="647" spans="1:3">
+      <c r="A647" t="s">
+        <v>553</v>
+      </c>
+      <c r="B647" t="s">
+        <v>683</v>
+      </c>
+      <c r="C647" t="s">
+        <v>564</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E1">
     <sortState ref="A2:E578">
@@ -23857,642 +26043,650 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B341">
+    <cfRule type="duplicateValues" dxfId="323" priority="337"/>
+    <cfRule type="duplicateValues" dxfId="322" priority="338"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B372">
+    <cfRule type="duplicateValues" dxfId="321" priority="335"/>
+    <cfRule type="duplicateValues" dxfId="320" priority="336"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B373">
     <cfRule type="duplicateValues" dxfId="319" priority="333"/>
     <cfRule type="duplicateValues" dxfId="318" priority="334"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B372">
+  <conditionalFormatting sqref="B374">
     <cfRule type="duplicateValues" dxfId="317" priority="331"/>
     <cfRule type="duplicateValues" dxfId="316" priority="332"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B373">
+  <conditionalFormatting sqref="B375">
     <cfRule type="duplicateValues" dxfId="315" priority="329"/>
     <cfRule type="duplicateValues" dxfId="314" priority="330"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B374">
+  <conditionalFormatting sqref="B376">
     <cfRule type="duplicateValues" dxfId="313" priority="327"/>
     <cfRule type="duplicateValues" dxfId="312" priority="328"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B375">
+  <conditionalFormatting sqref="B377">
     <cfRule type="duplicateValues" dxfId="311" priority="325"/>
     <cfRule type="duplicateValues" dxfId="310" priority="326"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B376">
-    <cfRule type="duplicateValues" dxfId="309" priority="323"/>
-    <cfRule type="duplicateValues" dxfId="308" priority="324"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B377">
-    <cfRule type="duplicateValues" dxfId="307" priority="321"/>
-    <cfRule type="duplicateValues" dxfId="306" priority="322"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B379:B390">
-    <cfRule type="duplicateValues" dxfId="305" priority="317"/>
-    <cfRule type="duplicateValues" dxfId="304" priority="318"/>
+    <cfRule type="duplicateValues" dxfId="309" priority="321"/>
+    <cfRule type="duplicateValues" dxfId="308" priority="322"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B391">
+    <cfRule type="duplicateValues" dxfId="307" priority="317"/>
+    <cfRule type="duplicateValues" dxfId="306" priority="318"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B392">
+    <cfRule type="duplicateValues" dxfId="305" priority="315"/>
+    <cfRule type="duplicateValues" dxfId="304" priority="316"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B393">
     <cfRule type="duplicateValues" dxfId="303" priority="313"/>
     <cfRule type="duplicateValues" dxfId="302" priority="314"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B392">
+  <conditionalFormatting sqref="B394">
     <cfRule type="duplicateValues" dxfId="301" priority="311"/>
     <cfRule type="duplicateValues" dxfId="300" priority="312"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B393">
+  <conditionalFormatting sqref="B395">
     <cfRule type="duplicateValues" dxfId="299" priority="309"/>
     <cfRule type="duplicateValues" dxfId="298" priority="310"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B394">
-    <cfRule type="duplicateValues" dxfId="297" priority="307"/>
-    <cfRule type="duplicateValues" dxfId="296" priority="308"/>
+  <conditionalFormatting sqref="B370:B371">
+    <cfRule type="duplicateValues" dxfId="297" priority="305"/>
+    <cfRule type="duplicateValues" dxfId="296" priority="306"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B395">
-    <cfRule type="duplicateValues" dxfId="295" priority="305"/>
-    <cfRule type="duplicateValues" dxfId="294" priority="306"/>
+  <conditionalFormatting sqref="B369">
+    <cfRule type="duplicateValues" dxfId="295" priority="303"/>
+    <cfRule type="duplicateValues" dxfId="294" priority="304"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B370:B371">
+  <conditionalFormatting sqref="B407">
     <cfRule type="duplicateValues" dxfId="293" priority="301"/>
     <cfRule type="duplicateValues" dxfId="292" priority="302"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B369">
+  <conditionalFormatting sqref="B408">
     <cfRule type="duplicateValues" dxfId="291" priority="299"/>
     <cfRule type="duplicateValues" dxfId="290" priority="300"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B407">
+  <conditionalFormatting sqref="B409">
     <cfRule type="duplicateValues" dxfId="289" priority="297"/>
     <cfRule type="duplicateValues" dxfId="288" priority="298"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B408">
+  <conditionalFormatting sqref="B410:B411">
     <cfRule type="duplicateValues" dxfId="287" priority="295"/>
     <cfRule type="duplicateValues" dxfId="286" priority="296"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B409">
+  <conditionalFormatting sqref="B413">
     <cfRule type="duplicateValues" dxfId="285" priority="293"/>
     <cfRule type="duplicateValues" dxfId="284" priority="294"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B410:B411">
+  <conditionalFormatting sqref="B414">
     <cfRule type="duplicateValues" dxfId="283" priority="291"/>
     <cfRule type="duplicateValues" dxfId="282" priority="292"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B413">
+  <conditionalFormatting sqref="B415">
     <cfRule type="duplicateValues" dxfId="281" priority="289"/>
     <cfRule type="duplicateValues" dxfId="280" priority="290"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B414">
+  <conditionalFormatting sqref="B416">
     <cfRule type="duplicateValues" dxfId="279" priority="287"/>
     <cfRule type="duplicateValues" dxfId="278" priority="288"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B415">
+  <conditionalFormatting sqref="B417">
     <cfRule type="duplicateValues" dxfId="277" priority="285"/>
     <cfRule type="duplicateValues" dxfId="276" priority="286"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B416">
+  <conditionalFormatting sqref="B419">
     <cfRule type="duplicateValues" dxfId="275" priority="283"/>
     <cfRule type="duplicateValues" dxfId="274" priority="284"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B417">
+  <conditionalFormatting sqref="B420">
     <cfRule type="duplicateValues" dxfId="273" priority="281"/>
     <cfRule type="duplicateValues" dxfId="272" priority="282"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B419">
+  <conditionalFormatting sqref="B421">
     <cfRule type="duplicateValues" dxfId="271" priority="279"/>
     <cfRule type="duplicateValues" dxfId="270" priority="280"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B420">
+  <conditionalFormatting sqref="B422">
     <cfRule type="duplicateValues" dxfId="269" priority="277"/>
     <cfRule type="duplicateValues" dxfId="268" priority="278"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B421">
+  <conditionalFormatting sqref="B423">
     <cfRule type="duplicateValues" dxfId="267" priority="275"/>
     <cfRule type="duplicateValues" dxfId="266" priority="276"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B422">
+  <conditionalFormatting sqref="B424">
     <cfRule type="duplicateValues" dxfId="265" priority="273"/>
     <cfRule type="duplicateValues" dxfId="264" priority="274"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B423">
+  <conditionalFormatting sqref="B425">
     <cfRule type="duplicateValues" dxfId="263" priority="271"/>
     <cfRule type="duplicateValues" dxfId="262" priority="272"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B424">
+  <conditionalFormatting sqref="B426">
     <cfRule type="duplicateValues" dxfId="261" priority="269"/>
     <cfRule type="duplicateValues" dxfId="260" priority="270"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B425">
+  <conditionalFormatting sqref="B418">
     <cfRule type="duplicateValues" dxfId="259" priority="267"/>
     <cfRule type="duplicateValues" dxfId="258" priority="268"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B426">
+  <conditionalFormatting sqref="B427">
     <cfRule type="duplicateValues" dxfId="257" priority="265"/>
     <cfRule type="duplicateValues" dxfId="256" priority="266"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B418">
+  <conditionalFormatting sqref="B428">
     <cfRule type="duplicateValues" dxfId="255" priority="263"/>
     <cfRule type="duplicateValues" dxfId="254" priority="264"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B427">
+  <conditionalFormatting sqref="B429">
     <cfRule type="duplicateValues" dxfId="253" priority="261"/>
     <cfRule type="duplicateValues" dxfId="252" priority="262"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B428">
+  <conditionalFormatting sqref="B430">
     <cfRule type="duplicateValues" dxfId="251" priority="259"/>
     <cfRule type="duplicateValues" dxfId="250" priority="260"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B429">
+  <conditionalFormatting sqref="B431">
     <cfRule type="duplicateValues" dxfId="249" priority="257"/>
     <cfRule type="duplicateValues" dxfId="248" priority="258"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B430">
+  <conditionalFormatting sqref="B432">
     <cfRule type="duplicateValues" dxfId="247" priority="255"/>
     <cfRule type="duplicateValues" dxfId="246" priority="256"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B431">
+  <conditionalFormatting sqref="B433">
     <cfRule type="duplicateValues" dxfId="245" priority="253"/>
     <cfRule type="duplicateValues" dxfId="244" priority="254"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B432">
+  <conditionalFormatting sqref="B434">
     <cfRule type="duplicateValues" dxfId="243" priority="251"/>
     <cfRule type="duplicateValues" dxfId="242" priority="252"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B433">
+  <conditionalFormatting sqref="B435">
     <cfRule type="duplicateValues" dxfId="241" priority="249"/>
     <cfRule type="duplicateValues" dxfId="240" priority="250"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B434">
+  <conditionalFormatting sqref="B436">
     <cfRule type="duplicateValues" dxfId="239" priority="247"/>
     <cfRule type="duplicateValues" dxfId="238" priority="248"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B435">
+  <conditionalFormatting sqref="B437">
     <cfRule type="duplicateValues" dxfId="237" priority="245"/>
     <cfRule type="duplicateValues" dxfId="236" priority="246"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B436">
+  <conditionalFormatting sqref="B438">
     <cfRule type="duplicateValues" dxfId="235" priority="243"/>
     <cfRule type="duplicateValues" dxfId="234" priority="244"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B437">
+  <conditionalFormatting sqref="B439">
     <cfRule type="duplicateValues" dxfId="233" priority="241"/>
     <cfRule type="duplicateValues" dxfId="232" priority="242"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B438">
+  <conditionalFormatting sqref="B440">
     <cfRule type="duplicateValues" dxfId="231" priority="239"/>
     <cfRule type="duplicateValues" dxfId="230" priority="240"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B439">
+  <conditionalFormatting sqref="B441">
     <cfRule type="duplicateValues" dxfId="229" priority="237"/>
     <cfRule type="duplicateValues" dxfId="228" priority="238"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B440">
+  <conditionalFormatting sqref="B442">
     <cfRule type="duplicateValues" dxfId="227" priority="235"/>
     <cfRule type="duplicateValues" dxfId="226" priority="236"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B441">
+  <conditionalFormatting sqref="B443">
     <cfRule type="duplicateValues" dxfId="225" priority="233"/>
     <cfRule type="duplicateValues" dxfId="224" priority="234"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B442">
+  <conditionalFormatting sqref="B444">
     <cfRule type="duplicateValues" dxfId="223" priority="231"/>
     <cfRule type="duplicateValues" dxfId="222" priority="232"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B443">
+  <conditionalFormatting sqref="B445">
     <cfRule type="duplicateValues" dxfId="221" priority="229"/>
     <cfRule type="duplicateValues" dxfId="220" priority="230"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B444">
+  <conditionalFormatting sqref="B446">
     <cfRule type="duplicateValues" dxfId="219" priority="227"/>
     <cfRule type="duplicateValues" dxfId="218" priority="228"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B445">
+  <conditionalFormatting sqref="B447">
     <cfRule type="duplicateValues" dxfId="217" priority="225"/>
     <cfRule type="duplicateValues" dxfId="216" priority="226"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B446">
+  <conditionalFormatting sqref="B448">
     <cfRule type="duplicateValues" dxfId="215" priority="223"/>
     <cfRule type="duplicateValues" dxfId="214" priority="224"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B447">
+  <conditionalFormatting sqref="B449">
     <cfRule type="duplicateValues" dxfId="213" priority="221"/>
     <cfRule type="duplicateValues" dxfId="212" priority="222"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B448">
+  <conditionalFormatting sqref="B450">
     <cfRule type="duplicateValues" dxfId="211" priority="219"/>
     <cfRule type="duplicateValues" dxfId="210" priority="220"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B449">
+  <conditionalFormatting sqref="B451">
     <cfRule type="duplicateValues" dxfId="209" priority="217"/>
     <cfRule type="duplicateValues" dxfId="208" priority="218"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B450">
+  <conditionalFormatting sqref="B452">
     <cfRule type="duplicateValues" dxfId="207" priority="215"/>
     <cfRule type="duplicateValues" dxfId="206" priority="216"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B451">
+  <conditionalFormatting sqref="B453">
     <cfRule type="duplicateValues" dxfId="205" priority="213"/>
     <cfRule type="duplicateValues" dxfId="204" priority="214"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B452">
+  <conditionalFormatting sqref="B454">
     <cfRule type="duplicateValues" dxfId="203" priority="211"/>
     <cfRule type="duplicateValues" dxfId="202" priority="212"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B453">
+  <conditionalFormatting sqref="B455">
     <cfRule type="duplicateValues" dxfId="201" priority="209"/>
     <cfRule type="duplicateValues" dxfId="200" priority="210"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B454">
+  <conditionalFormatting sqref="B456">
     <cfRule type="duplicateValues" dxfId="199" priority="207"/>
     <cfRule type="duplicateValues" dxfId="198" priority="208"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B455">
+  <conditionalFormatting sqref="B457">
     <cfRule type="duplicateValues" dxfId="197" priority="205"/>
     <cfRule type="duplicateValues" dxfId="196" priority="206"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B456">
+  <conditionalFormatting sqref="B458">
     <cfRule type="duplicateValues" dxfId="195" priority="203"/>
     <cfRule type="duplicateValues" dxfId="194" priority="204"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B457">
+  <conditionalFormatting sqref="B459">
     <cfRule type="duplicateValues" dxfId="193" priority="201"/>
     <cfRule type="duplicateValues" dxfId="192" priority="202"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B458">
+  <conditionalFormatting sqref="B460">
     <cfRule type="duplicateValues" dxfId="191" priority="199"/>
     <cfRule type="duplicateValues" dxfId="190" priority="200"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B459">
+  <conditionalFormatting sqref="B461">
     <cfRule type="duplicateValues" dxfId="189" priority="197"/>
     <cfRule type="duplicateValues" dxfId="188" priority="198"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B460">
+  <conditionalFormatting sqref="B462">
     <cfRule type="duplicateValues" dxfId="187" priority="195"/>
     <cfRule type="duplicateValues" dxfId="186" priority="196"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B461">
+  <conditionalFormatting sqref="B463">
     <cfRule type="duplicateValues" dxfId="185" priority="193"/>
     <cfRule type="duplicateValues" dxfId="184" priority="194"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B462">
+  <conditionalFormatting sqref="B464">
     <cfRule type="duplicateValues" dxfId="183" priority="191"/>
     <cfRule type="duplicateValues" dxfId="182" priority="192"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B463">
+  <conditionalFormatting sqref="B465">
     <cfRule type="duplicateValues" dxfId="181" priority="189"/>
     <cfRule type="duplicateValues" dxfId="180" priority="190"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B464">
+  <conditionalFormatting sqref="B466:B467">
     <cfRule type="duplicateValues" dxfId="179" priority="187"/>
     <cfRule type="duplicateValues" dxfId="178" priority="188"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B465">
+  <conditionalFormatting sqref="B468">
     <cfRule type="duplicateValues" dxfId="177" priority="185"/>
     <cfRule type="duplicateValues" dxfId="176" priority="186"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B466:B467">
+  <conditionalFormatting sqref="B469">
     <cfRule type="duplicateValues" dxfId="175" priority="183"/>
     <cfRule type="duplicateValues" dxfId="174" priority="184"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B468">
+  <conditionalFormatting sqref="B470">
     <cfRule type="duplicateValues" dxfId="173" priority="181"/>
     <cfRule type="duplicateValues" dxfId="172" priority="182"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B469">
+  <conditionalFormatting sqref="B471">
     <cfRule type="duplicateValues" dxfId="171" priority="179"/>
     <cfRule type="duplicateValues" dxfId="170" priority="180"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B470">
+  <conditionalFormatting sqref="B472">
     <cfRule type="duplicateValues" dxfId="169" priority="177"/>
     <cfRule type="duplicateValues" dxfId="168" priority="178"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B471">
+  <conditionalFormatting sqref="B473">
     <cfRule type="duplicateValues" dxfId="167" priority="175"/>
     <cfRule type="duplicateValues" dxfId="166" priority="176"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B472">
-    <cfRule type="duplicateValues" dxfId="165" priority="173"/>
-    <cfRule type="duplicateValues" dxfId="164" priority="174"/>
+  <conditionalFormatting sqref="B474">
+    <cfRule type="duplicateValues" dxfId="165" priority="171"/>
+    <cfRule type="duplicateValues" dxfId="164" priority="172"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B473">
-    <cfRule type="duplicateValues" dxfId="163" priority="171"/>
-    <cfRule type="duplicateValues" dxfId="162" priority="172"/>
+  <conditionalFormatting sqref="B475">
+    <cfRule type="duplicateValues" dxfId="163" priority="169"/>
+    <cfRule type="duplicateValues" dxfId="162" priority="170"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B474">
+  <conditionalFormatting sqref="B476">
     <cfRule type="duplicateValues" dxfId="161" priority="167"/>
     <cfRule type="duplicateValues" dxfId="160" priority="168"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B475">
+  <conditionalFormatting sqref="B477">
     <cfRule type="duplicateValues" dxfId="159" priority="165"/>
     <cfRule type="duplicateValues" dxfId="158" priority="166"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B476">
+  <conditionalFormatting sqref="B478">
     <cfRule type="duplicateValues" dxfId="157" priority="163"/>
     <cfRule type="duplicateValues" dxfId="156" priority="164"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B477">
+  <conditionalFormatting sqref="B479">
     <cfRule type="duplicateValues" dxfId="155" priority="161"/>
     <cfRule type="duplicateValues" dxfId="154" priority="162"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B478">
+  <conditionalFormatting sqref="B480">
     <cfRule type="duplicateValues" dxfId="153" priority="159"/>
     <cfRule type="duplicateValues" dxfId="152" priority="160"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B479">
+  <conditionalFormatting sqref="B481">
     <cfRule type="duplicateValues" dxfId="151" priority="157"/>
     <cfRule type="duplicateValues" dxfId="150" priority="158"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B480">
+  <conditionalFormatting sqref="B482">
     <cfRule type="duplicateValues" dxfId="149" priority="155"/>
     <cfRule type="duplicateValues" dxfId="148" priority="156"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B481">
+  <conditionalFormatting sqref="B483">
     <cfRule type="duplicateValues" dxfId="147" priority="153"/>
     <cfRule type="duplicateValues" dxfId="146" priority="154"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B482">
+  <conditionalFormatting sqref="B489">
     <cfRule type="duplicateValues" dxfId="145" priority="151"/>
     <cfRule type="duplicateValues" dxfId="144" priority="152"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B483">
+  <conditionalFormatting sqref="B490:B491">
     <cfRule type="duplicateValues" dxfId="143" priority="149"/>
     <cfRule type="duplicateValues" dxfId="142" priority="150"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B489">
+  <conditionalFormatting sqref="B492">
     <cfRule type="duplicateValues" dxfId="141" priority="147"/>
     <cfRule type="duplicateValues" dxfId="140" priority="148"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B490:B491">
+  <conditionalFormatting sqref="B493">
     <cfRule type="duplicateValues" dxfId="139" priority="145"/>
     <cfRule type="duplicateValues" dxfId="138" priority="146"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B492">
+  <conditionalFormatting sqref="B494">
     <cfRule type="duplicateValues" dxfId="137" priority="143"/>
     <cfRule type="duplicateValues" dxfId="136" priority="144"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B493">
+  <conditionalFormatting sqref="B495">
     <cfRule type="duplicateValues" dxfId="135" priority="141"/>
     <cfRule type="duplicateValues" dxfId="134" priority="142"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B494">
+  <conditionalFormatting sqref="B496">
     <cfRule type="duplicateValues" dxfId="133" priority="139"/>
     <cfRule type="duplicateValues" dxfId="132" priority="140"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B495">
+  <conditionalFormatting sqref="B497">
     <cfRule type="duplicateValues" dxfId="131" priority="137"/>
     <cfRule type="duplicateValues" dxfId="130" priority="138"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B496">
+  <conditionalFormatting sqref="B498">
     <cfRule type="duplicateValues" dxfId="129" priority="135"/>
     <cfRule type="duplicateValues" dxfId="128" priority="136"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B497">
+  <conditionalFormatting sqref="B499">
     <cfRule type="duplicateValues" dxfId="127" priority="133"/>
     <cfRule type="duplicateValues" dxfId="126" priority="134"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B498">
+  <conditionalFormatting sqref="B500">
     <cfRule type="duplicateValues" dxfId="125" priority="131"/>
     <cfRule type="duplicateValues" dxfId="124" priority="132"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B499">
+  <conditionalFormatting sqref="B501">
     <cfRule type="duplicateValues" dxfId="123" priority="129"/>
     <cfRule type="duplicateValues" dxfId="122" priority="130"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B500">
+  <conditionalFormatting sqref="B502">
     <cfRule type="duplicateValues" dxfId="121" priority="127"/>
     <cfRule type="duplicateValues" dxfId="120" priority="128"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B501">
+  <conditionalFormatting sqref="B503">
     <cfRule type="duplicateValues" dxfId="119" priority="125"/>
     <cfRule type="duplicateValues" dxfId="118" priority="126"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B502">
+  <conditionalFormatting sqref="B504">
     <cfRule type="duplicateValues" dxfId="117" priority="123"/>
     <cfRule type="duplicateValues" dxfId="116" priority="124"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B503">
+  <conditionalFormatting sqref="B505">
     <cfRule type="duplicateValues" dxfId="115" priority="121"/>
     <cfRule type="duplicateValues" dxfId="114" priority="122"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B504">
+  <conditionalFormatting sqref="B506">
     <cfRule type="duplicateValues" dxfId="113" priority="119"/>
     <cfRule type="duplicateValues" dxfId="112" priority="120"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B505">
+  <conditionalFormatting sqref="B507">
     <cfRule type="duplicateValues" dxfId="111" priority="117"/>
     <cfRule type="duplicateValues" dxfId="110" priority="118"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B506">
+  <conditionalFormatting sqref="B508">
     <cfRule type="duplicateValues" dxfId="109" priority="115"/>
     <cfRule type="duplicateValues" dxfId="108" priority="116"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B507">
+  <conditionalFormatting sqref="B509">
     <cfRule type="duplicateValues" dxfId="107" priority="113"/>
     <cfRule type="duplicateValues" dxfId="106" priority="114"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B508">
+  <conditionalFormatting sqref="B510">
     <cfRule type="duplicateValues" dxfId="105" priority="111"/>
     <cfRule type="duplicateValues" dxfId="104" priority="112"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B509">
+  <conditionalFormatting sqref="B511">
     <cfRule type="duplicateValues" dxfId="103" priority="109"/>
     <cfRule type="duplicateValues" dxfId="102" priority="110"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B510">
+  <conditionalFormatting sqref="B512">
     <cfRule type="duplicateValues" dxfId="101" priority="107"/>
     <cfRule type="duplicateValues" dxfId="100" priority="108"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B511">
+  <conditionalFormatting sqref="B513">
     <cfRule type="duplicateValues" dxfId="99" priority="105"/>
     <cfRule type="duplicateValues" dxfId="98" priority="106"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B512">
+  <conditionalFormatting sqref="B514">
     <cfRule type="duplicateValues" dxfId="97" priority="103"/>
     <cfRule type="duplicateValues" dxfId="96" priority="104"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B513">
+  <conditionalFormatting sqref="B515">
     <cfRule type="duplicateValues" dxfId="95" priority="101"/>
     <cfRule type="duplicateValues" dxfId="94" priority="102"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B514">
+  <conditionalFormatting sqref="B516">
     <cfRule type="duplicateValues" dxfId="93" priority="99"/>
     <cfRule type="duplicateValues" dxfId="92" priority="100"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B515">
+  <conditionalFormatting sqref="B517">
     <cfRule type="duplicateValues" dxfId="91" priority="97"/>
     <cfRule type="duplicateValues" dxfId="90" priority="98"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B516">
+  <conditionalFormatting sqref="B518">
     <cfRule type="duplicateValues" dxfId="89" priority="95"/>
     <cfRule type="duplicateValues" dxfId="88" priority="96"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B517">
+  <conditionalFormatting sqref="B519">
     <cfRule type="duplicateValues" dxfId="87" priority="93"/>
     <cfRule type="duplicateValues" dxfId="86" priority="94"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B518">
+  <conditionalFormatting sqref="B520">
     <cfRule type="duplicateValues" dxfId="85" priority="91"/>
     <cfRule type="duplicateValues" dxfId="84" priority="92"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B519">
+  <conditionalFormatting sqref="B521">
     <cfRule type="duplicateValues" dxfId="83" priority="89"/>
     <cfRule type="duplicateValues" dxfId="82" priority="90"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B520">
+  <conditionalFormatting sqref="B522">
     <cfRule type="duplicateValues" dxfId="81" priority="87"/>
     <cfRule type="duplicateValues" dxfId="80" priority="88"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B521">
+  <conditionalFormatting sqref="B523">
     <cfRule type="duplicateValues" dxfId="79" priority="85"/>
     <cfRule type="duplicateValues" dxfId="78" priority="86"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B522">
+  <conditionalFormatting sqref="B524">
     <cfRule type="duplicateValues" dxfId="77" priority="83"/>
     <cfRule type="duplicateValues" dxfId="76" priority="84"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B523">
+  <conditionalFormatting sqref="B525">
     <cfRule type="duplicateValues" dxfId="75" priority="81"/>
     <cfRule type="duplicateValues" dxfId="74" priority="82"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B524">
+  <conditionalFormatting sqref="B526">
     <cfRule type="duplicateValues" dxfId="73" priority="79"/>
     <cfRule type="duplicateValues" dxfId="72" priority="80"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B525">
+  <conditionalFormatting sqref="B527">
     <cfRule type="duplicateValues" dxfId="71" priority="77"/>
     <cfRule type="duplicateValues" dxfId="70" priority="78"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B526">
+  <conditionalFormatting sqref="B528">
     <cfRule type="duplicateValues" dxfId="69" priority="75"/>
     <cfRule type="duplicateValues" dxfId="68" priority="76"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B527">
+  <conditionalFormatting sqref="A528">
     <cfRule type="duplicateValues" dxfId="67" priority="73"/>
     <cfRule type="duplicateValues" dxfId="66" priority="74"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B528">
+  <conditionalFormatting sqref="B529">
     <cfRule type="duplicateValues" dxfId="65" priority="71"/>
     <cfRule type="duplicateValues" dxfId="64" priority="72"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A528">
+  <conditionalFormatting sqref="B530">
     <cfRule type="duplicateValues" dxfId="63" priority="69"/>
     <cfRule type="duplicateValues" dxfId="62" priority="70"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B529">
+  <conditionalFormatting sqref="B531">
     <cfRule type="duplicateValues" dxfId="61" priority="67"/>
     <cfRule type="duplicateValues" dxfId="60" priority="68"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B530">
+  <conditionalFormatting sqref="B532">
     <cfRule type="duplicateValues" dxfId="59" priority="65"/>
     <cfRule type="duplicateValues" dxfId="58" priority="66"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B531">
+  <conditionalFormatting sqref="A532">
     <cfRule type="duplicateValues" dxfId="57" priority="63"/>
     <cfRule type="duplicateValues" dxfId="56" priority="64"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B532">
+  <conditionalFormatting sqref="B533">
     <cfRule type="duplicateValues" dxfId="55" priority="61"/>
     <cfRule type="duplicateValues" dxfId="54" priority="62"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A532">
+  <conditionalFormatting sqref="B534">
     <cfRule type="duplicateValues" dxfId="53" priority="59"/>
     <cfRule type="duplicateValues" dxfId="52" priority="60"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B533">
+  <conditionalFormatting sqref="B535">
     <cfRule type="duplicateValues" dxfId="51" priority="57"/>
     <cfRule type="duplicateValues" dxfId="50" priority="58"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B534">
+  <conditionalFormatting sqref="B536:B537">
     <cfRule type="duplicateValues" dxfId="49" priority="55"/>
     <cfRule type="duplicateValues" dxfId="48" priority="56"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B535">
+  <conditionalFormatting sqref="B538:B539">
     <cfRule type="duplicateValues" dxfId="47" priority="53"/>
     <cfRule type="duplicateValues" dxfId="46" priority="54"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B536:B537">
+  <conditionalFormatting sqref="A539">
     <cfRule type="duplicateValues" dxfId="45" priority="51"/>
     <cfRule type="duplicateValues" dxfId="44" priority="52"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B538:B539">
+  <conditionalFormatting sqref="B540">
     <cfRule type="duplicateValues" dxfId="43" priority="49"/>
     <cfRule type="duplicateValues" dxfId="42" priority="50"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A539">
+  <conditionalFormatting sqref="A540">
     <cfRule type="duplicateValues" dxfId="41" priority="47"/>
     <cfRule type="duplicateValues" dxfId="40" priority="48"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B540">
+  <conditionalFormatting sqref="B541">
     <cfRule type="duplicateValues" dxfId="39" priority="45"/>
     <cfRule type="duplicateValues" dxfId="38" priority="46"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A540">
+  <conditionalFormatting sqref="B542:B543">
     <cfRule type="duplicateValues" dxfId="37" priority="43"/>
     <cfRule type="duplicateValues" dxfId="36" priority="44"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B541">
+  <conditionalFormatting sqref="A543">
     <cfRule type="duplicateValues" dxfId="35" priority="41"/>
     <cfRule type="duplicateValues" dxfId="34" priority="42"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B542:B543">
+  <conditionalFormatting sqref="B544">
     <cfRule type="duplicateValues" dxfId="33" priority="39"/>
     <cfRule type="duplicateValues" dxfId="32" priority="40"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A543">
+  <conditionalFormatting sqref="B545">
     <cfRule type="duplicateValues" dxfId="31" priority="37"/>
     <cfRule type="duplicateValues" dxfId="30" priority="38"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B544">
+  <conditionalFormatting sqref="B546">
     <cfRule type="duplicateValues" dxfId="29" priority="35"/>
     <cfRule type="duplicateValues" dxfId="28" priority="36"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B545">
+  <conditionalFormatting sqref="A553">
     <cfRule type="duplicateValues" dxfId="27" priority="33"/>
     <cfRule type="duplicateValues" dxfId="26" priority="34"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B546">
+  <conditionalFormatting sqref="B559">
     <cfRule type="duplicateValues" dxfId="25" priority="31"/>
     <cfRule type="duplicateValues" dxfId="24" priority="32"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A553">
-    <cfRule type="duplicateValues" dxfId="23" priority="29"/>
-    <cfRule type="duplicateValues" dxfId="22" priority="30"/>
+  <conditionalFormatting sqref="A548">
+    <cfRule type="duplicateValues" dxfId="23" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="26"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B559">
-    <cfRule type="duplicateValues" dxfId="21" priority="27"/>
-    <cfRule type="duplicateValues" dxfId="20" priority="28"/>
+  <conditionalFormatting sqref="B564:B565">
+    <cfRule type="duplicateValues" dxfId="21" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="24"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A548">
+  <conditionalFormatting sqref="B567">
     <cfRule type="duplicateValues" dxfId="19" priority="21"/>
     <cfRule type="duplicateValues" dxfId="18" priority="22"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B564:B565">
+  <conditionalFormatting sqref="A569">
     <cfRule type="duplicateValues" dxfId="17" priority="19"/>
     <cfRule type="duplicateValues" dxfId="16" priority="20"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B567">
+  <conditionalFormatting sqref="B572">
     <cfRule type="duplicateValues" dxfId="15" priority="17"/>
     <cfRule type="duplicateValues" dxfId="14" priority="18"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A569">
+  <conditionalFormatting sqref="A572">
     <cfRule type="duplicateValues" dxfId="13" priority="15"/>
     <cfRule type="duplicateValues" dxfId="12" priority="16"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B572">
+  <conditionalFormatting sqref="B576">
     <cfRule type="duplicateValues" dxfId="11" priority="13"/>
     <cfRule type="duplicateValues" dxfId="10" priority="14"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A572">
+  <conditionalFormatting sqref="A576">
     <cfRule type="duplicateValues" dxfId="9" priority="11"/>
     <cfRule type="duplicateValues" dxfId="8" priority="12"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B576">
-    <cfRule type="duplicateValues" dxfId="7" priority="9"/>
-    <cfRule type="duplicateValues" dxfId="6" priority="10"/>
+  <conditionalFormatting sqref="B577">
+    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A576">
-    <cfRule type="duplicateValues" dxfId="5" priority="7"/>
-    <cfRule type="duplicateValues" dxfId="4" priority="8"/>
+  <conditionalFormatting sqref="B578">
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B577">
+  <conditionalFormatting sqref="B579">
     <cfRule type="duplicateValues" dxfId="3" priority="3"/>
     <cfRule type="duplicateValues" dxfId="2" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B578">
+  <conditionalFormatting sqref="B580">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>

</xml_diff>